<commit_message>
archivos funcionando, se agrega clusterizacion UNEs
</commit_message>
<xml_diff>
--- a/Resultados/Lista_unique_UNEs.xlsx
+++ b/Resultados/Lista_unique_UNEs.xlsx
@@ -450,21 +450,21 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>D003</t>
+          <t>D002</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>D002</t>
+          <t>D004</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>D004</t>
+          <t>D003</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
se agrega db_backup_test, todos los scripts funcionando
</commit_message>
<xml_diff>
--- a/Resultados/Lista_unique_UNEs.xlsx
+++ b/Resultados/Lista_unique_UNEs.xlsx
@@ -450,21 +450,21 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>D002</t>
+          <t>D004</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>D004</t>
+          <t>D003</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>D003</t>
+          <t>D002</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
se agrega script db_backup_test, para subir parquets a cloud
</commit_message>
<xml_diff>
--- a/Resultados/Lista_unique_UNEs.xlsx
+++ b/Resultados/Lista_unique_UNEs.xlsx
@@ -450,7 +450,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>D004</t>
+          <t>D002</t>
         </is>
       </c>
     </row>
@@ -464,7 +464,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>D002</t>
+          <t>D004</t>
         </is>
       </c>
     </row>

</xml_diff>